<commit_message>
flexible execution; 3 operators: FILL; ClICK; FIND(YES/NOT).
</commit_message>
<xml_diff>
--- a/formstest/webFillExсel.xlsx
+++ b/formstest/webFillExсel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t xml:space="preserve">ID NO. </t>
   </si>
@@ -23,22 +23,31 @@
     <t>web_url</t>
   </si>
   <si>
-    <t>field1_xpass</t>
-  </si>
-  <si>
-    <t>field1_content</t>
-  </si>
-  <si>
-    <t>field2_xpass</t>
-  </si>
-  <si>
-    <t>field2_content</t>
-  </si>
-  <si>
-    <t>field3_xpass</t>
-  </si>
-  <si>
-    <t>field3_content</t>
+    <t>operator1</t>
+  </si>
+  <si>
+    <t>rXpath1</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>operator2</t>
+  </si>
+  <si>
+    <t>rXpath2</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>operator3</t>
+  </si>
+  <si>
+    <t>subfunc3</t>
+  </si>
+  <si>
+    <t>text3</t>
   </si>
   <si>
     <t>my_web1</t>
@@ -55,25 +64,34 @@
     </r>
   </si>
   <si>
-    <t>xpass1_text1</t>
-  </si>
-  <si>
-    <t>field1_text1</t>
-  </si>
-  <si>
-    <t>xpass2_text1</t>
-  </si>
-  <si>
-    <t>field2_text2</t>
-  </si>
-  <si>
-    <t>xpass3_text1</t>
-  </si>
-  <si>
-    <t>field3_text1</t>
-  </si>
-  <si>
-    <t>google</t>
+    <t>FILL</t>
+  </si>
+  <si>
+    <t>rXpath1_web1</t>
+  </si>
+  <si>
+    <t>text1_web1</t>
+  </si>
+  <si>
+    <t>CLICK</t>
+  </si>
+  <si>
+    <t>rXpath2_web1</t>
+  </si>
+  <si>
+    <t>text2_web1</t>
+  </si>
+  <si>
+    <t>FIND</t>
+  </si>
+  <si>
+    <t>subfunc3_web1</t>
+  </si>
+  <si>
+    <t>text3_web1</t>
+  </si>
+  <si>
+    <t>yahoo</t>
   </si>
   <si>
     <r>
@@ -96,13 +114,10 @@
     <t>//button[@id='uh-search-button']</t>
   </si>
   <si>
-    <t>click()</t>
-  </si>
-  <si>
-    <t>NO: No item found matching your search criteria.</t>
-  </si>
-  <si>
-    <t>found</t>
+    <t>text2_web2</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
   <si>
     <t>estate</t>
@@ -122,13 +137,22 @@
     <t>//form[@name='frm_search']/input[@name='s']</t>
   </si>
   <si>
-    <t>christmas tree</t>
+    <t>Christmas tree</t>
   </si>
   <si>
     <t>//form[@name='frm_search']/input[@value='search']</t>
   </si>
   <si>
-    <t>my_web4</t>
+    <t>text2_web3</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>dkslfjksdh</t>
+  </si>
+  <si>
+    <t>my_web5</t>
   </si>
   <si>
     <r>
@@ -142,190 +166,169 @@
     </r>
   </si>
   <si>
-    <t>xpass1_text4</t>
-  </si>
-  <si>
-    <t>field1_text4</t>
-  </si>
-  <si>
-    <t>xpass2_text4</t>
-  </si>
-  <si>
-    <t>field2_text5</t>
-  </si>
-  <si>
-    <t>xpass3_text4</t>
-  </si>
-  <si>
-    <t>field3_text4</t>
-  </si>
-  <si>
-    <t>my_web5</t>
-  </si>
-  <si>
-    <t>xpass1_text5</t>
-  </si>
-  <si>
-    <t>field1_text5</t>
-  </si>
-  <si>
-    <t>xpass2_text5</t>
-  </si>
-  <si>
-    <t>field2_text6</t>
-  </si>
-  <si>
-    <t>xpass3_text5</t>
-  </si>
-  <si>
-    <t>field3_text5</t>
+    <t>rXpath1_web5</t>
+  </si>
+  <si>
+    <t>text1_web5</t>
+  </si>
+  <si>
+    <t>rXpath2_web5</t>
+  </si>
+  <si>
+    <t>text2_web5</t>
+  </si>
+  <si>
+    <t>subfunc3_text5</t>
+  </si>
+  <si>
+    <t>text3_web5</t>
   </si>
   <si>
     <t>my_web6</t>
   </si>
   <si>
-    <t>xpass1_text6</t>
-  </si>
-  <si>
-    <t>field1_text6</t>
-  </si>
-  <si>
-    <t>xpass2_text6</t>
-  </si>
-  <si>
-    <t>field2_text7</t>
-  </si>
-  <si>
-    <t>xpass3_text6</t>
-  </si>
-  <si>
-    <t>field3_text6</t>
+    <t>rXpath1_web6</t>
+  </si>
+  <si>
+    <t>text1_web6</t>
+  </si>
+  <si>
+    <t>rXpath2_web6</t>
+  </si>
+  <si>
+    <t>text2_web6</t>
+  </si>
+  <si>
+    <t>subfunc3_text6</t>
+  </si>
+  <si>
+    <t>text3_web6</t>
   </si>
   <si>
     <t>my_web7</t>
   </si>
   <si>
-    <t>xpass1_text7</t>
-  </si>
-  <si>
-    <t>field1_text7</t>
-  </si>
-  <si>
-    <t>xpass2_text7</t>
-  </si>
-  <si>
-    <t>field2_text8</t>
-  </si>
-  <si>
-    <t>xpass3_text7</t>
-  </si>
-  <si>
-    <t>field3_text7</t>
+    <t>rXpath1_web7</t>
+  </si>
+  <si>
+    <t>text1_web7</t>
+  </si>
+  <si>
+    <t>rXpath2_web7</t>
+  </si>
+  <si>
+    <t>text2_web7</t>
+  </si>
+  <si>
+    <t>subfunc3_text7</t>
+  </si>
+  <si>
+    <t>text3_web7</t>
   </si>
   <si>
     <t>my_web8</t>
   </si>
   <si>
-    <t>xpass1_text8</t>
-  </si>
-  <si>
-    <t>field1_text8</t>
-  </si>
-  <si>
-    <t>xpass2_text8</t>
-  </si>
-  <si>
-    <t>field2_text9</t>
-  </si>
-  <si>
-    <t>xpass3_text8</t>
-  </si>
-  <si>
-    <t>field3_text8</t>
+    <t>rXpath1_web8</t>
+  </si>
+  <si>
+    <t>text1_web8</t>
+  </si>
+  <si>
+    <t>rXpath2_web8</t>
+  </si>
+  <si>
+    <t>text2_web8</t>
+  </si>
+  <si>
+    <t>subfunc3_text8</t>
+  </si>
+  <si>
+    <t>text3_web8</t>
   </si>
   <si>
     <t>my_web9</t>
   </si>
   <si>
-    <t>xpass1_text9</t>
-  </si>
-  <si>
-    <t>field1_text9</t>
-  </si>
-  <si>
-    <t>xpass2_text9</t>
-  </si>
-  <si>
-    <t>field2_text10</t>
-  </si>
-  <si>
-    <t>xpass3_text9</t>
-  </si>
-  <si>
-    <t>field3_text9</t>
+    <t>rXpath1_web9</t>
+  </si>
+  <si>
+    <t>text1_web9</t>
+  </si>
+  <si>
+    <t>rXpath2_web9</t>
+  </si>
+  <si>
+    <t>text2_web9</t>
+  </si>
+  <si>
+    <t>subfunc3_text9</t>
+  </si>
+  <si>
+    <t>text3_web9</t>
   </si>
   <si>
     <t>my_web10</t>
   </si>
   <si>
-    <t>xpass1_text10</t>
-  </si>
-  <si>
-    <t>field1_text10</t>
-  </si>
-  <si>
-    <t>xpass2_text10</t>
-  </si>
-  <si>
-    <t>field2_text11</t>
-  </si>
-  <si>
-    <t>xpass3_text10</t>
-  </si>
-  <si>
-    <t>field3_text10</t>
+    <t>rXpath1_web10</t>
+  </si>
+  <si>
+    <t>text1_web10</t>
+  </si>
+  <si>
+    <t>rXpath2_web10</t>
+  </si>
+  <si>
+    <t>text2_web10</t>
+  </si>
+  <si>
+    <t>subfunc3_text10</t>
+  </si>
+  <si>
+    <t>text3_web10</t>
   </si>
   <si>
     <t>my_web11</t>
   </si>
   <si>
-    <t>xpass1_text11</t>
-  </si>
-  <si>
-    <t>field1_text11</t>
-  </si>
-  <si>
-    <t>xpass2_text11</t>
-  </si>
-  <si>
-    <t>field2_text12</t>
-  </si>
-  <si>
-    <t>xpass3_text11</t>
-  </si>
-  <si>
-    <t>field3_text11</t>
+    <t>rXpath1_web11</t>
+  </si>
+  <si>
+    <t>text1_web11</t>
+  </si>
+  <si>
+    <t>rXpath2_web11</t>
+  </si>
+  <si>
+    <t>text2_web11</t>
+  </si>
+  <si>
+    <t>subfunc3_text11</t>
+  </si>
+  <si>
+    <t>text3_web11</t>
   </si>
   <si>
     <t>my_web12</t>
   </si>
   <si>
-    <t>xpass1_text12</t>
-  </si>
-  <si>
-    <t>field1_text12</t>
-  </si>
-  <si>
-    <t>xpass2_text12</t>
-  </si>
-  <si>
-    <t>field2_text13</t>
-  </si>
-  <si>
-    <t>xpass3_text12</t>
-  </si>
-  <si>
-    <t>field3_text12</t>
+    <t>rXpath1_web12</t>
+  </si>
+  <si>
+    <t>text1_web12</t>
+  </si>
+  <si>
+    <t>rXpath2_web12</t>
+  </si>
+  <si>
+    <t>text2_web12</t>
+  </si>
+  <si>
+    <t>subfunc3_text12</t>
+  </si>
+  <si>
+    <t>text3_web12</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1633,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1639,11 +1642,15 @@
     <col min="1" max="1" width="7.04688" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.0234" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.9219" style="1" customWidth="1"/>
-    <col min="7" max="9" width="16.3516" style="1" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4297" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.8359" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85156" style="1" customWidth="1"/>
+    <col min="11" max="12" width="16.3516" style="1" customWidth="1"/>
+    <col min="13" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1674,34 +1681,52 @@
       <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s" s="6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s" s="6">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="6">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s" s="6">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="J2" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s" s="6">
+        <v>22</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
@@ -1709,28 +1734,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C3" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="10">
+      <c r="H3" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s" s="10">
         <v>20</v>
       </c>
-      <c r="F3" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s" s="10">
-        <v>24</v>
+      <c r="K3" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s" s="10">
+        <v>26</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
@@ -1738,28 +1772,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="8">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s" s="9">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s" s="10">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s" s="10">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s" s="10">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s" s="10">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s" s="10">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s" s="10">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="J4" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s" s="10">
+        <v>37</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
@@ -1773,22 +1816,31 @@
         <v>31</v>
       </c>
       <c r="D5" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="10">
         <v>32</v>
       </c>
-      <c r="E5" t="s" s="10">
+      <c r="F5" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="G5" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s" s="10">
         <v>34</v>
       </c>
-      <c r="G5" t="s" s="10">
+      <c r="I5" t="s" s="10">
         <v>35</v>
       </c>
-      <c r="H5" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="I5" t="s" s="10">
-        <v>37</v>
+      <c r="J5" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="L5" t="s" s="10">
+        <v>33</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
@@ -1799,10 +1851,10 @@
         <v>38</v>
       </c>
       <c r="C6" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s" s="10">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s" s="10">
         <v>40</v>
@@ -1811,13 +1863,22 @@
         <v>41</v>
       </c>
       <c r="G6" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s" s="10">
         <v>42</v>
       </c>
-      <c r="H6" t="s" s="10">
+      <c r="I6" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="I6" t="s" s="10">
+      <c r="J6" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s" s="10">
         <v>44</v>
+      </c>
+      <c r="L6" t="s" s="10">
+        <v>45</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
@@ -1825,13 +1886,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="8">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s" s="10">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s" s="10">
         <v>47</v>
@@ -1840,13 +1901,22 @@
         <v>48</v>
       </c>
       <c r="G7" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s" s="10">
         <v>49</v>
       </c>
-      <c r="H7" t="s" s="10">
+      <c r="I7" t="s" s="10">
         <v>50</v>
       </c>
-      <c r="I7" t="s" s="10">
+      <c r="J7" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s" s="10">
         <v>51</v>
+      </c>
+      <c r="L7" t="s" s="10">
+        <v>52</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
@@ -1854,13 +1924,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s" s="10">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s" s="10">
         <v>54</v>
@@ -1869,13 +1939,22 @@
         <v>55</v>
       </c>
       <c r="G8" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s" s="10">
         <v>56</v>
       </c>
-      <c r="H8" t="s" s="10">
+      <c r="I8" t="s" s="10">
         <v>57</v>
       </c>
-      <c r="I8" t="s" s="10">
+      <c r="J8" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s" s="10">
         <v>58</v>
+      </c>
+      <c r="L8" t="s" s="10">
+        <v>59</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
@@ -1883,13 +1962,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="8">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s" s="10">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s" s="10">
         <v>61</v>
@@ -1898,13 +1977,22 @@
         <v>62</v>
       </c>
       <c r="G9" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s" s="10">
         <v>63</v>
       </c>
-      <c r="H9" t="s" s="10">
+      <c r="I9" t="s" s="10">
         <v>64</v>
       </c>
-      <c r="I9" t="s" s="10">
+      <c r="J9" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s" s="10">
         <v>65</v>
+      </c>
+      <c r="L9" t="s" s="10">
+        <v>66</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
@@ -1912,13 +2000,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="8">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s" s="10">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s" s="10">
         <v>68</v>
@@ -1927,13 +2015,22 @@
         <v>69</v>
       </c>
       <c r="G10" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s" s="10">
         <v>70</v>
       </c>
-      <c r="H10" t="s" s="10">
+      <c r="I10" t="s" s="10">
         <v>71</v>
       </c>
-      <c r="I10" t="s" s="10">
+      <c r="J10" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s" s="10">
         <v>72</v>
+      </c>
+      <c r="L10" t="s" s="10">
+        <v>73</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
@@ -1941,13 +2038,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="8">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s" s="10">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s" s="10">
         <v>75</v>
@@ -1956,13 +2053,22 @@
         <v>76</v>
       </c>
       <c r="G11" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s" s="10">
         <v>77</v>
       </c>
-      <c r="H11" t="s" s="10">
+      <c r="I11" t="s" s="10">
         <v>78</v>
       </c>
-      <c r="I11" t="s" s="10">
+      <c r="J11" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K11" t="s" s="10">
         <v>79</v>
+      </c>
+      <c r="L11" t="s" s="10">
+        <v>80</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
@@ -1970,13 +2076,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="8">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s" s="10">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s" s="10">
         <v>82</v>
@@ -1985,13 +2091,22 @@
         <v>83</v>
       </c>
       <c r="G12" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s" s="10">
         <v>84</v>
       </c>
-      <c r="H12" t="s" s="10">
+      <c r="I12" t="s" s="10">
         <v>85</v>
       </c>
-      <c r="I12" t="s" s="10">
+      <c r="J12" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s" s="10">
         <v>86</v>
+      </c>
+      <c r="L12" t="s" s="10">
+        <v>87</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
@@ -1999,13 +2114,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="8">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s" s="9">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s" s="10">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s" s="10">
         <v>89</v>
@@ -2014,13 +2129,22 @@
         <v>90</v>
       </c>
       <c r="G13" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s" s="10">
         <v>91</v>
       </c>
-      <c r="H13" t="s" s="10">
+      <c r="I13" t="s" s="10">
         <v>92</v>
       </c>
-      <c r="I13" t="s" s="10">
+      <c r="J13" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s" s="10">
         <v>93</v>
+      </c>
+      <c r="L13" t="s" s="10">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Process 1 line with No. or all lines with choice of 0.
</commit_message>
<xml_diff>
--- a/formstest/webFillExсel.xlsx
+++ b/formstest/webFillExсel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t xml:space="preserve">ID NO. </t>
   </si>
@@ -48,47 +48,6 @@
   </si>
   <si>
     <t>text3</t>
-  </si>
-  <si>
-    <t>my_web1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>www.my_web1.com</t>
-    </r>
-  </si>
-  <si>
-    <t>FILL</t>
-  </si>
-  <si>
-    <t>rXpath1_web1</t>
-  </si>
-  <si>
-    <t>text1_web1</t>
-  </si>
-  <si>
-    <t>CLICK</t>
-  </si>
-  <si>
-    <t>rXpath2_web1</t>
-  </si>
-  <si>
-    <t>text2_web1</t>
-  </si>
-  <si>
-    <t>FIND</t>
-  </si>
-  <si>
-    <t>subfunc3_web1</t>
-  </si>
-  <si>
-    <t>text3_web1</t>
   </si>
   <si>
     <t>yahoo</t>
@@ -105,16 +64,25 @@
     </r>
   </si>
   <si>
+    <t>FILL</t>
+  </si>
+  <si>
     <t>//input[@id='uh-search-box']</t>
   </si>
   <si>
     <t xml:space="preserve">what’s up? </t>
   </si>
   <si>
+    <t>CLICK</t>
+  </si>
+  <si>
     <t>//button[@id='uh-search-button']</t>
   </si>
   <si>
     <t>text2_web2</t>
+  </si>
+  <si>
+    <t>FIND</t>
   </si>
   <si>
     <t>YES</t>
@@ -150,185 +118,6 @@
   </si>
   <si>
     <t>dkslfjksdh</t>
-  </si>
-  <si>
-    <t>my_web5</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>www.my_web4.com</t>
-    </r>
-  </si>
-  <si>
-    <t>rXpath1_web5</t>
-  </si>
-  <si>
-    <t>text1_web5</t>
-  </si>
-  <si>
-    <t>rXpath2_web5</t>
-  </si>
-  <si>
-    <t>text2_web5</t>
-  </si>
-  <si>
-    <t>subfunc3_text5</t>
-  </si>
-  <si>
-    <t>text3_web5</t>
-  </si>
-  <si>
-    <t>my_web6</t>
-  </si>
-  <si>
-    <t>rXpath1_web6</t>
-  </si>
-  <si>
-    <t>text1_web6</t>
-  </si>
-  <si>
-    <t>rXpath2_web6</t>
-  </si>
-  <si>
-    <t>text2_web6</t>
-  </si>
-  <si>
-    <t>subfunc3_text6</t>
-  </si>
-  <si>
-    <t>text3_web6</t>
-  </si>
-  <si>
-    <t>my_web7</t>
-  </si>
-  <si>
-    <t>rXpath1_web7</t>
-  </si>
-  <si>
-    <t>text1_web7</t>
-  </si>
-  <si>
-    <t>rXpath2_web7</t>
-  </si>
-  <si>
-    <t>text2_web7</t>
-  </si>
-  <si>
-    <t>subfunc3_text7</t>
-  </si>
-  <si>
-    <t>text3_web7</t>
-  </si>
-  <si>
-    <t>my_web8</t>
-  </si>
-  <si>
-    <t>rXpath1_web8</t>
-  </si>
-  <si>
-    <t>text1_web8</t>
-  </si>
-  <si>
-    <t>rXpath2_web8</t>
-  </si>
-  <si>
-    <t>text2_web8</t>
-  </si>
-  <si>
-    <t>subfunc3_text8</t>
-  </si>
-  <si>
-    <t>text3_web8</t>
-  </si>
-  <si>
-    <t>my_web9</t>
-  </si>
-  <si>
-    <t>rXpath1_web9</t>
-  </si>
-  <si>
-    <t>text1_web9</t>
-  </si>
-  <si>
-    <t>rXpath2_web9</t>
-  </si>
-  <si>
-    <t>text2_web9</t>
-  </si>
-  <si>
-    <t>subfunc3_text9</t>
-  </si>
-  <si>
-    <t>text3_web9</t>
-  </si>
-  <si>
-    <t>my_web10</t>
-  </si>
-  <si>
-    <t>rXpath1_web10</t>
-  </si>
-  <si>
-    <t>text1_web10</t>
-  </si>
-  <si>
-    <t>rXpath2_web10</t>
-  </si>
-  <si>
-    <t>text2_web10</t>
-  </si>
-  <si>
-    <t>subfunc3_text10</t>
-  </si>
-  <si>
-    <t>text3_web10</t>
-  </si>
-  <si>
-    <t>my_web11</t>
-  </si>
-  <si>
-    <t>rXpath1_web11</t>
-  </si>
-  <si>
-    <t>text1_web11</t>
-  </si>
-  <si>
-    <t>rXpath2_web11</t>
-  </si>
-  <si>
-    <t>text2_web11</t>
-  </si>
-  <si>
-    <t>subfunc3_text11</t>
-  </si>
-  <si>
-    <t>text3_web11</t>
-  </si>
-  <si>
-    <t>my_web12</t>
-  </si>
-  <si>
-    <t>rXpath1_web12</t>
-  </si>
-  <si>
-    <t>text1_web12</t>
-  </si>
-  <si>
-    <t>rXpath2_web12</t>
-  </si>
-  <si>
-    <t>text2_web12</t>
-  </si>
-  <si>
-    <t>subfunc3_text12</t>
-  </si>
-  <si>
-    <t>text3_web12</t>
   </si>
 </sst>
 </file>
@@ -393,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -421,6 +210,21 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -439,7 +243,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -467,36 +271,6 @@
       </left>
       <right style="thin">
         <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -512,7 +286,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -522,29 +296,26 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1633,7 +1404,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1657,19 +1428,19 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
       <c r="G1" t="s" s="2">
@@ -1687,464 +1458,122 @@
       <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" t="s" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E2" t="s" s="6">
+      <c r="E2" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="G2" t="s" s="6">
+      <c r="G2" t="s" s="8">
         <v>17</v>
       </c>
-      <c r="H2" t="s" s="6">
+      <c r="H2" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="I2" t="s" s="6">
+      <c r="I2" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="J2" t="s" s="6">
+      <c r="J2" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="K2" t="s" s="6">
+      <c r="K2" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="L2" t="s" s="6">
-        <v>22</v>
+      <c r="L2" t="s" s="7">
+        <v>16</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s" s="6">
         <v>23</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="D3" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="D3" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s" s="10">
+      <c r="F3" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="G3" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="G3" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s" s="10">
+      <c r="I3" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="I3" t="s" s="10">
+      <c r="J3" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s" s="7">
         <v>28</v>
       </c>
-      <c r="J3" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s" s="10">
+      <c r="L3" t="s" s="7">
         <v>29</v>
-      </c>
-      <c r="L3" t="s" s="10">
-        <v>26</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="7">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s" s="10">
+      <c r="B4" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="E4" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s" s="10">
+      <c r="E4" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="H4" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s" s="10">
+      <c r="H4" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="K4" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="L4" t="s" s="10">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="L5" t="s" s="10">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s" s="10">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s" s="10">
-        <v>42</v>
-      </c>
-      <c r="I6" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="L6" t="s" s="10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="8">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s" s="10">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s" s="10">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s" s="10">
-        <v>49</v>
-      </c>
-      <c r="I7" t="s" s="10">
-        <v>50</v>
-      </c>
-      <c r="J7" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K7" t="s" s="10">
-        <v>51</v>
-      </c>
-      <c r="L7" t="s" s="10">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="8">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s" s="10">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s" s="10">
-        <v>55</v>
-      </c>
-      <c r="G8" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s" s="10">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s" s="10">
-        <v>57</v>
-      </c>
-      <c r="J8" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K8" t="s" s="10">
-        <v>58</v>
-      </c>
-      <c r="L8" t="s" s="10">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s" s="8">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s" s="10">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s" s="10">
-        <v>62</v>
-      </c>
-      <c r="G9" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s" s="10">
-        <v>63</v>
-      </c>
-      <c r="I9" t="s" s="10">
-        <v>64</v>
-      </c>
-      <c r="J9" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s" s="10">
-        <v>65</v>
-      </c>
-      <c r="L9" t="s" s="10">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s" s="8">
-        <v>67</v>
-      </c>
-      <c r="C10" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s" s="10">
-        <v>68</v>
-      </c>
-      <c r="F10" t="s" s="10">
-        <v>69</v>
-      </c>
-      <c r="G10" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s" s="10">
-        <v>70</v>
-      </c>
-      <c r="I10" t="s" s="10">
-        <v>71</v>
-      </c>
-      <c r="J10" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K10" t="s" s="10">
-        <v>72</v>
-      </c>
-      <c r="L10" t="s" s="10">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s" s="8">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s" s="10">
-        <v>75</v>
-      </c>
-      <c r="F11" t="s" s="10">
-        <v>76</v>
-      </c>
-      <c r="G11" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s" s="10">
-        <v>77</v>
-      </c>
-      <c r="I11" t="s" s="10">
-        <v>78</v>
-      </c>
-      <c r="J11" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K11" t="s" s="10">
-        <v>79</v>
-      </c>
-      <c r="L11" t="s" s="10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="C12" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s" s="10">
-        <v>82</v>
-      </c>
-      <c r="F12" t="s" s="10">
-        <v>83</v>
-      </c>
-      <c r="G12" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s" s="10">
-        <v>84</v>
-      </c>
-      <c r="I12" t="s" s="10">
-        <v>85</v>
-      </c>
-      <c r="J12" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K12" t="s" s="10">
-        <v>86</v>
-      </c>
-      <c r="L12" t="s" s="10">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s" s="8">
-        <v>88</v>
-      </c>
-      <c r="C13" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s" s="10">
-        <v>89</v>
-      </c>
-      <c r="F13" t="s" s="10">
-        <v>90</v>
-      </c>
-      <c r="G13" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s" s="10">
-        <v>91</v>
-      </c>
-      <c r="I13" t="s" s="10">
-        <v>92</v>
-      </c>
-      <c r="J13" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="K13" t="s" s="10">
-        <v>93</v>
-      </c>
-      <c r="L13" t="s" s="10">
-        <v>94</v>
+      <c r="K4" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s" s="7">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2152,15 +1581,6 @@
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display=""/>
     <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display=""/>
-    <hyperlink ref="C5" r:id="rId4" location="" tooltip="" display=""/>
-    <hyperlink ref="C6" r:id="rId5" location="" tooltip="" display=""/>
-    <hyperlink ref="C7" r:id="rId6" location="" tooltip="" display=""/>
-    <hyperlink ref="C8" r:id="rId7" location="" tooltip="" display=""/>
-    <hyperlink ref="C9" r:id="rId8" location="" tooltip="" display=""/>
-    <hyperlink ref="C10" r:id="rId9" location="" tooltip="" display=""/>
-    <hyperlink ref="C11" r:id="rId10" location="" tooltip="" display=""/>
-    <hyperlink ref="C12" r:id="rId11" location="" tooltip="" display=""/>
-    <hyperlink ref="C13" r:id="rId12" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Submit action operator added.
</commit_message>
<xml_diff>
--- a/formstest/webFillExсel.xlsx
+++ b/formstest/webFillExсel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t xml:space="preserve">ID NO. </t>
   </si>
@@ -118,6 +118,32 @@
   </si>
   <si>
     <t>dkslfjksdh</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://google.com</t>
+    </r>
+  </si>
+  <si>
+    <t>SBMT</t>
+  </si>
+  <si>
+    <t>//input[@id='lst-ib']</t>
+  </si>
+  <si>
+    <t>What is the weather in Dallas today?</t>
+  </si>
+  <si>
+    <t>Dallas</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1430,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1420,7 +1446,8 @@
     <col min="8" max="8" width="13.8359" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.85156" style="1" customWidth="1"/>
-    <col min="11" max="12" width="16.3516" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.99219" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7891" style="1" customWidth="1"/>
     <col min="13" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1576,11 +1603,50 @@
         <v>25</v>
       </c>
     </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s" s="7">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display=""/>
     <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="C5" r:id="rId4" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>